<commit_message>
Update OPL with tasks from Kick-Off-Meeting
</commit_message>
<xml_diff>
--- a/Projekthandbuch/Planungsdokumente/Offene_Punkteliste.xlsx
+++ b/Projekthandbuch/Planungsdokumente/Offene_Punkteliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i589151/repos/webengineering/Projekthandbuch/Planungsdokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F7704AD-D06B-8C4F-A963-C93FE3090497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F1A9AB-4328-0F4A-8E43-3E459FD44090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPL Vorlage" sheetId="9" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Nr.</t>
   </si>
@@ -96,9 +96,6 @@
   <si>
     <t>zu
 erledigen bis</t>
-  </si>
-  <si>
-    <t>Merkel</t>
   </si>
   <si>
     <r>
@@ -310,21 +307,6 @@
     <t>alle</t>
   </si>
   <si>
-    <t>Thomas A.</t>
-  </si>
-  <si>
-    <t>Frauke B.</t>
-  </si>
-  <si>
-    <t>Sabine K.</t>
-  </si>
-  <si>
-    <t>Michael O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN: </t>
-  </si>
-  <si>
     <t>Kick-Off-Meeting</t>
   </si>
   <si>
@@ -335,6 +317,18 @@
   </si>
   <si>
     <t>Marius Kurth</t>
+  </si>
+  <si>
+    <t>POC der APIs</t>
+  </si>
+  <si>
+    <t>Details s. Protokoll 15.05.2024</t>
+  </si>
+  <si>
+    <t>bis 24.05.2024</t>
+  </si>
+  <si>
+    <t>Design-Entwurf</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1479,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -1510,7 +1504,7 @@
     <row r="1" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22"/>
       <c r="B1" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
@@ -1527,13 +1521,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>2</v>
@@ -1557,13 +1551,13 @@
     </row>
     <row r="3" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="26"/>
@@ -1571,62 +1565,82 @@
         <v>45427</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="10"/>
       <c r="N3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A4" s="20"/>
       <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="27"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="25"/>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>13</v>
+      </c>
       <c r="J4" s="10"/>
       <c r="N4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A5" s="20"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="E5" s="27"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="J5" s="10"/>
       <c r="N5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
@@ -1640,13 +1654,13 @@
       <c r="H6" s="3"/>
       <c r="J6" s="10"/>
       <c r="N6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
@@ -2340,7 +2354,7 @@
   <dimension ref="C1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2351,38 +2365,34 @@
   <sheetData>
     <row r="1" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C1" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C3" s="8" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C5" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C6" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C8" s="8"/>
@@ -2445,20 +2455,81 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ed3b3e4c-9488-4b1c-9f3e-6d18d478a7c3" ContentTypeId="0x010100DA2BCA46EDEB4642AC63457AE234917801" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Value>6</Value>
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>8</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <g160457a8c434834a5b53f659fe1e746 xmlns="14aa5bc9-86d3-4ab5-8fe5-a5dc8f7f2173">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Nicht zugeordnet</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c303b6eb-4f10-4121-a11e-bafbaa8ed95e</TermId>
+        </TermInfo>
+      </Terms>
+    </g160457a8c434834a5b53f659fe1e746>
+    <UIT_Projektnummer xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">1936</UIT_Projektnummer>
+    <TaxKeywordTaxHTField xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <d432c6d2d8d844e782d3944c98e74891 xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">C1</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">21a0c8e3-ddb0-46ee-ba05-3f67ebc4c672</TermId>
+        </TermInfo>
+      </Terms>
+    </d432c6d2d8d844e782d3944c98e74891>
+    <ifc6eb3f52e649b3b934c6ee22f60e94 xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Stäbe/IT</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">918b0a6e-6c10-4e87-b691-15d7a93b48c1</TermId>
+        </TermInfo>
+      </Terms>
+    </ifc6eb3f52e649b3b934c6ee22f60e94>
+    <UIT_Projektstatus xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">Umsetzung aktiv</UIT_Projektstatus>
+    <ffeb0ce8d0664cc682573a89f4df646c xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Infrastruktur</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">84b02811-c171-46ba-9c59-667d2612ca5f</TermId>
+        </TermInfo>
+      </Terms>
+    </ffeb0ce8d0664cc682573a89f4df646c>
+    <Dokumentenstatus xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">offen</Dokumentenstatus>
+    <me67adabb15c4c469550ce34f167698b xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Projekte</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4650438d-5fcd-44f4-ac37-1249f2cd8809</TermId>
+        </TermInfo>
+      </Terms>
+    </me67adabb15c4c469550ce34f167698b>
+    <UIT_Projektkoordinator xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <UserInfo>
+        <DisplayName>Hoeppener, Joachim (UIT)</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </UIT_Projektkoordinator>
+    <UIT_Projektkurzname xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">WorkIn</UIT_Projektkurzname>
+    <UIT_Projektleitung xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
+      <UserInfo>
+        <DisplayName>Merkel, Frank (UIT)</DisplayName>
+        <AccountId>9</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </UIT_Projektleitung>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Arbeitsdokument" ma:contentTypeID="0x010100DA2BCA46EDEB4642AC63457AE234917801002B0616426A3BB54080A66203D35FA55B" ma:contentTypeVersion="8" ma:contentTypeDescription="Inhaltstyp für Arbeitsdokumente im Projektraum" ma:contentTypeScope="" ma:versionID="6b9379cda9ace72b012619bd3b59ca51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="369aca94-4c50-4928-9ca5-72dc029195ff" xmlns:ns3="14aa5bc9-86d3-4ab5-8fe5-a5dc8f7f2173" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32c192c1efd5bead4b33c440147ce62c" ns2:_="" ns3:_="">
     <xsd:import namespace="369aca94-4c50-4928-9ca5-72dc029195ff"/>
@@ -2736,98 +2807,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Value>6</Value>
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>8</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <g160457a8c434834a5b53f659fe1e746 xmlns="14aa5bc9-86d3-4ab5-8fe5-a5dc8f7f2173">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Nicht zugeordnet</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c303b6eb-4f10-4121-a11e-bafbaa8ed95e</TermId>
-        </TermInfo>
-      </Terms>
-    </g160457a8c434834a5b53f659fe1e746>
-    <UIT_Projektnummer xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">1936</UIT_Projektnummer>
-    <TaxKeywordTaxHTField xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <d432c6d2d8d844e782d3944c98e74891 xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">C1</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">21a0c8e3-ddb0-46ee-ba05-3f67ebc4c672</TermId>
-        </TermInfo>
-      </Terms>
-    </d432c6d2d8d844e782d3944c98e74891>
-    <ifc6eb3f52e649b3b934c6ee22f60e94 xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Stäbe/IT</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">918b0a6e-6c10-4e87-b691-15d7a93b48c1</TermId>
-        </TermInfo>
-      </Terms>
-    </ifc6eb3f52e649b3b934c6ee22f60e94>
-    <UIT_Projektstatus xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">Umsetzung aktiv</UIT_Projektstatus>
-    <ffeb0ce8d0664cc682573a89f4df646c xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Infrastruktur</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">84b02811-c171-46ba-9c59-667d2612ca5f</TermId>
-        </TermInfo>
-      </Terms>
-    </ffeb0ce8d0664cc682573a89f4df646c>
-    <Dokumentenstatus xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">offen</Dokumentenstatus>
-    <me67adabb15c4c469550ce34f167698b xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Projekte</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4650438d-5fcd-44f4-ac37-1249f2cd8809</TermId>
-        </TermInfo>
-      </Terms>
-    </me67adabb15c4c469550ce34f167698b>
-    <UIT_Projektkoordinator xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <UserInfo>
-        <DisplayName>Hoeppener, Joachim (UIT)</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </UIT_Projektkoordinator>
-    <UIT_Projektkurzname xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">WorkIn</UIT_Projektkurzname>
-    <UIT_Projektleitung xmlns="369aca94-4c50-4928-9ca5-72dc029195ff">
-      <UserInfo>
-        <DisplayName>Merkel, Frank (UIT)</DisplayName>
-        <AccountId>9</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </UIT_Projektleitung>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ed3b3e4c-9488-4b1c-9f3e-6d18d478a7c3" ContentTypeId="0x010100DA2BCA46EDEB4642AC63457AE234917801" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25B2B0E0-C5C4-4A25-ACB1-2FBEE9393F67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1C35BC-27AA-41CF-9154-D8424654DF68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="14aa5bc9-86d3-4ab5-8fe5-a5dc8f7f2173"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="369aca94-4c50-4928-9ca5-72dc029195ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60EB098D-9F34-4534-AA48-089EB13C9C50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13DB965-66FA-42E5-AABB-31E5CE688967}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2846,19 +2857,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60EB098D-9F34-4534-AA48-089EB13C9C50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1C35BC-27AA-41CF-9154-D8424654DF68}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25B2B0E0-C5C4-4A25-ACB1-2FBEE9393F67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="14aa5bc9-86d3-4ab5-8fe5-a5dc8f7f2173"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="369aca94-4c50-4928-9ca5-72dc029195ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>